<commit_message>
before modify merge kline jump
</commit_message>
<xml_diff>
--- a/src/main/resources/SZ300181.xlsx
+++ b/src/main/resources/SZ300181.xlsx
@@ -68,577 +68,577 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>782.0</v>
+        <v>780.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20151021</t>
+          <t>20151125</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>882.0</v>
+        <v>1254.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20151116</t>
+          <t>20151211</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1026.0</v>
+        <v>1055.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20151125</t>
+          <t>20151223</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1256.0</v>
+        <v>1283.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20151211</t>
+          <t>20160129</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1057.0</v>
+        <v>783.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20151223</t>
+          <t>20160222</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1285.0</v>
+        <v>965.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20160129</t>
+          <t>20160229</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>785.0</v>
+        <v>745.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20160222</t>
+          <t>20160321</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>967.0</v>
+        <v>907.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20160229</t>
+          <t>20160329</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>747.0</v>
+        <v>837.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20160321</t>
+          <t>20160412</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>909.0</v>
+        <v>1029.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20160329</t>
+          <t>20160425</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>839.0</v>
+        <v>860.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20160412</t>
+          <t>20160503</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1031.0</v>
+        <v>953.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20160425</t>
+          <t>20160520</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>862.0</v>
+        <v>787.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20160503</t>
+          <t>20160727</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>955.0</v>
+        <v>985.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20160520</t>
+          <t>20160801</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>789.0</v>
+        <v>862.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20160727</t>
+          <t>20161012</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>987.0</v>
+        <v>1054.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20160801</t>
+          <t>20161021</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>864.0</v>
+        <v>971.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20161012</t>
+          <t>20161118</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1056.0</v>
+        <v>1151.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20161021</t>
+          <t>20170116</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>973.0</v>
+        <v>786.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20161118</t>
+          <t>20170208</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1153.0</v>
+        <v>910.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20170116</t>
+          <t>20170511</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>788.0</v>
+        <v>643.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20170208</t>
+          <t>20170710</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>912.0</v>
+        <v>711.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20170511</t>
+          <t>20170724</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>645.0</v>
+        <v>612.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20170710</t>
+          <t>20170907</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>713.0</v>
+        <v>787.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20170724</t>
+          <t>20170922</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>614.0</v>
+        <v>695.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20170907</t>
+          <t>20171011</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>789.0</v>
+        <v>756.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20170922</t>
+          <t>20171103</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>697.0</v>
+        <v>624.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20171011</t>
+          <t>20171117</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>758.0</v>
+        <v>678.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20171103</t>
+          <t>20171206</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>626.0</v>
+        <v>566.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20171117</t>
+          <t>20171226</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>680.0</v>
+        <v>837.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20171206</t>
+          <t>20180207</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>568.0</v>
+        <v>528.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20171226</t>
+          <t>20180314</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>839.0</v>
+        <v>746.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20180207</t>
+          <t>20180326</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>530.0</v>
+        <v>594.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20180314</t>
+          <t>20180402</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>748.0</v>
+        <v>791.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20180326</t>
+          <t>20180423</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>596.0</v>
+        <v>609.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20180402</t>
+          <t>20180524</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>793.0</v>
+        <v>723.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20180423</t>
+          <t>20180709</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>611.0</v>
+        <v>477.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20180524</t>
+          <t>20180725</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>725.0</v>
+        <v>535.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20180709</t>
+          <t>20180903</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>479.0</v>
+        <v>415.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20180725</t>
+          <t>20180926</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>537.0</v>
+        <v>467.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20180903</t>
+          <t>20181019</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>417.0</v>
+        <v>323.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20180926</t>
+          <t>20181204</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>469.0</v>
+        <v>676.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20181019</t>
+          <t>20190131</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>325.0</v>
+        <v>447.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20181204</t>
+          <t>20190325</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>678.0</v>
+        <v>847.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20190131</t>
+          <t>20190506</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>449.0</v>
+        <v>544.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20190325</t>
+          <t>20190528</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>849.0</v>
+        <v>657.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20190506</t>
+          <t>20190610</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>546.0</v>
+        <v>566.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20190528</t>
+          <t>20190621</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>659.0</v>
+        <v>635.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20190610</t>
+          <t>20190722</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>568.0</v>
+        <v>532.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20190621</t>
+          <t>20190731</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>637.0</v>
+        <v>566.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20190722</t>
+          <t>20190806</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>534.0</v>
+        <v>468.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20190731</t>
+          <t>20190910</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>568.0</v>
+        <v>583.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20190806</t>
+          <t>20200203</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>470.0</v>
+        <v>462.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20190910</t>
+          <t>20200327</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>585.0</v>
+        <v>666.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20200203</t>
+          <t>20200402</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>464.0</v>
+        <v>526.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20200327</t>
+          <t>20200416</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>668.0</v>
+        <v>625.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20200402</t>
+          <t>20200428</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>528.0</v>
+        <v>523.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>20200416</t>
+          <t>20200603</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>627.0</v>
+        <v>598.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
left containe error fix
</commit_message>
<xml_diff>
--- a/src/main/resources/SZ300181.xlsx
+++ b/src/main/resources/SZ300181.xlsx
@@ -64,581 +64,411 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>20150918</t>
+          <t>20170904</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>780.0</v>
+        <v>3433.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20151125</t>
+          <t>20170929</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1254.0</v>
+        <v>2308.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20151211</t>
+          <t>20171013</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1055.0</v>
+        <v>2934.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20151223</t>
+          <t>20171206</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1283.0</v>
+        <v>1728.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20160129</t>
+          <t>20171228</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>783.0</v>
+        <v>1993.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20160222</t>
+          <t>20180108</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>965.0</v>
+        <v>1844.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20160229</t>
+          <t>20180116</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>745.0</v>
+        <v>2148.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20160321</t>
+          <t>20180207</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>907.0</v>
+        <v>1376.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20160329</t>
+          <t>20180312</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>837.0</v>
+        <v>1718.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20160412</t>
+          <t>20180326</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1029.0</v>
+        <v>1431.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20160520</t>
+          <t>20180413</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>787.0</v>
+        <v>2022.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20160617</t>
+          <t>20180423</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>941.0</v>
+        <v>1671.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20160624</t>
+          <t>20180528</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>849.0</v>
+        <v>2289.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20160727</t>
+          <t>20180706</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>985.0</v>
+        <v>1482.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20160801</t>
+          <t>20180713</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>862.0</v>
+        <v>1737.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20161012</t>
+          <t>20180824</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1054.0</v>
+        <v>1383.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20161021</t>
+          <t>20180912</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>971.0</v>
+        <v>1520.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20161118</t>
+          <t>20181012</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1151.0</v>
+        <v>1124.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20170116</t>
+          <t>20181113</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>786.0</v>
+        <v>1485.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20170208</t>
+          <t>20181126</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>910.0</v>
+        <v>1323.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20170511</t>
+          <t>20181211</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>643.0</v>
+        <v>1941.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20170710</t>
+          <t>20181228</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>711.0</v>
+        <v>1622.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20170724</t>
+          <t>20190109</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>612.0</v>
+        <v>2041.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20170907</t>
+          <t>20190130</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>787.0</v>
+        <v>1642.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20170922</t>
+          <t>20190225</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>695.0</v>
+        <v>1968.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20171011</t>
+          <t>20190311</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>756.0</v>
+        <v>1692.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20171103</t>
+          <t>20190319</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>624.0</v>
+        <v>2216.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20171117</t>
+          <t>20190606</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>678.0</v>
+        <v>1430.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20171206</t>
+          <t>20190724</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>566.0</v>
+        <v>1808.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20171226</t>
+          <t>20190812</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>837.0</v>
+        <v>1383.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20180207</t>
+          <t>20191121</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>528.0</v>
+        <v>3392.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20180314</t>
+          <t>20191230</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>746.0</v>
+        <v>1680.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20180326</t>
+          <t>20200121</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>594.0</v>
+        <v>1865.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20180402</t>
+          <t>20200204</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>791.0</v>
+        <v>1355.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20180423</t>
+          <t>20200225</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>609.0</v>
+        <v>1978.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20180524</t>
+          <t>20200228</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>723.0</v>
+        <v>1651.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20180709</t>
+          <t>20200306</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>477.0</v>
+        <v>1845.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20180725</t>
+          <t>20200319</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>535.0</v>
+        <v>1451.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20180903</t>
+          <t>20200521</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>415.0</v>
+        <v>2700.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20180926</t>
+          <t>20200529</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>467.0</v>
+        <v>2015.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20181019</t>
+          <t>20200624</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>323.0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>20181204</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>676.0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>20190131</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
-        <v>447.0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>20190325</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>847.0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>20190506</t>
-        </is>
-      </c>
-      <c r="B45" t="n">
-        <v>544.0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>20190528</t>
-        </is>
-      </c>
-      <c r="B46" t="n">
-        <v>657.0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>20190610</t>
-        </is>
-      </c>
-      <c r="B47" t="n">
-        <v>566.0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>20190621</t>
-        </is>
-      </c>
-      <c r="B48" t="n">
-        <v>635.0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>20190722</t>
-        </is>
-      </c>
-      <c r="B49" t="n">
-        <v>532.0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>20190731</t>
-        </is>
-      </c>
-      <c r="B50" t="n">
-        <v>566.0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>20190806</t>
-        </is>
-      </c>
-      <c r="B51" t="n">
-        <v>468.0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>20190910</t>
-        </is>
-      </c>
-      <c r="B52" t="n">
-        <v>583.0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>20200203</t>
-        </is>
-      </c>
-      <c r="B53" t="n">
-        <v>462.0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>20200327</t>
-        </is>
-      </c>
-      <c r="B54" t="n">
-        <v>666.0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>20200402</t>
-        </is>
-      </c>
-      <c r="B55" t="n">
-        <v>526.0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>20200416</t>
-        </is>
-      </c>
-      <c r="B56" t="n">
-        <v>625.0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>20200428</t>
-        </is>
-      </c>
-      <c r="B57" t="n">
-        <v>523.0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>20200617</t>
-        </is>
-      </c>
-      <c r="B58" t="n">
-        <v>620.0</v>
+        <v>3230.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change jump and break point handle method order
</commit_message>
<xml_diff>
--- a/src/main/resources/SZ300181.xlsx
+++ b/src/main/resources/SZ300181.xlsx
@@ -64,590 +64,620 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>20150918</t>
+          <t>20150914</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>780.0</v>
+        <v>821.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20151125</t>
+          <t>20150918</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1254.0</v>
+        <v>780.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20151211</t>
+          <t>20151125</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1055.0</v>
+        <v>1254.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20151223</t>
+          <t>20151211</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1283.0</v>
+        <v>1055.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20160129</t>
+          <t>20151223</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>783.0</v>
+        <v>1283.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20160222</t>
+          <t>20160112</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>965.0</v>
+        <v>839.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20160229</t>
+          <t>20160222</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>745.0</v>
+        <v>965.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20160321</t>
+          <t>20160229</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>907.0</v>
+        <v>745.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20160329</t>
+          <t>20160321</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>837.0</v>
+        <v>907.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20160412</t>
+          <t>20160329</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1029.0</v>
+        <v>837.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20160520</t>
+          <t>20160412</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>787.0</v>
+        <v>1029.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20160617</t>
+          <t>20160520</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>941.0</v>
+        <v>787.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20160624</t>
+          <t>20160617</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>849.0</v>
+        <v>941.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20160727</t>
+          <t>20160624</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>985.0</v>
+        <v>849.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20160801</t>
+          <t>20160727</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>862.0</v>
+        <v>985.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20161012</t>
+          <t>20160801</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1054.0</v>
+        <v>862.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20161021</t>
+          <t>20161012</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>971.0</v>
+        <v>1054.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20161118</t>
+          <t>20161021</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1151.0</v>
+        <v>971.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20170116</t>
+          <t>20161118</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>786.0</v>
+        <v>1151.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20170208</t>
+          <t>20170116</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>910.0</v>
+        <v>786.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20170511</t>
+          <t>20170208</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>643.0</v>
+        <v>910.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20170710</t>
+          <t>20170511</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>711.0</v>
+        <v>643.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20170724</t>
+          <t>20170710</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>612.0</v>
+        <v>711.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20170907</t>
+          <t>20170724</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>787.0</v>
+        <v>612.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20170922</t>
+          <t>20170907</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>695.0</v>
+        <v>787.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20171011</t>
+          <t>20170922</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>756.0</v>
+        <v>695.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20171103</t>
+          <t>20171011</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>624.0</v>
+        <v>756.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20171117</t>
+          <t>20171103</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>678.0</v>
+        <v>624.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20171206</t>
+          <t>20171117</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>566.0</v>
+        <v>678.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20171226</t>
+          <t>20171206</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>837.0</v>
+        <v>566.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20180207</t>
+          <t>20171226</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>528.0</v>
+        <v>837.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20180314</t>
+          <t>20180207</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>746.0</v>
+        <v>528.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20180326</t>
+          <t>20180314</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>594.0</v>
+        <v>746.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20180402</t>
+          <t>20180326</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>791.0</v>
+        <v>594.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20180423</t>
+          <t>20180402</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>609.0</v>
+        <v>791.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20180524</t>
+          <t>20180423</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>723.0</v>
+        <v>609.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20180709</t>
+          <t>20180511</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>477.0</v>
+        <v>710.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20180725</t>
+          <t>20180709</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>535.0</v>
+        <v>477.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20180903</t>
+          <t>20180713</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>415.0</v>
+        <v>528.0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20180926</t>
+          <t>20180903</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>467.0</v>
+        <v>415.0</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20181019</t>
+          <t>20180926</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>323.0</v>
+        <v>467.0</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20181204</t>
+          <t>20181019</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>676.0</v>
+        <v>323.0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20190131</t>
+          <t>20181204</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>447.0</v>
+        <v>676.0</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20190325</t>
+          <t>20181218</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>847.0</v>
+        <v>470.0</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20190506</t>
+          <t>20190325</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>544.0</v>
+        <v>847.0</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20190528</t>
+          <t>20190506</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>657.0</v>
+        <v>544.0</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20190610</t>
+          <t>20190528</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>566.0</v>
+        <v>657.0</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20190621</t>
+          <t>20190610</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>635.0</v>
+        <v>566.0</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20190722</t>
+          <t>20190621</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>532.0</v>
+        <v>635.0</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20190731</t>
+          <t>20190722</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>566.0</v>
+        <v>532.0</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20190806</t>
+          <t>20190731</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>468.0</v>
+        <v>566.0</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>20190910</t>
+          <t>20190806</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>583.0</v>
+        <v>468.0</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20200203</t>
+          <t>20190910</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>462.0</v>
+        <v>583.0</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20200327</t>
+          <t>20191021</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>666.0</v>
+        <v>478.0</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20200402</t>
+          <t>20191105</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>526.0</v>
+        <v>538.0</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20200416</t>
+          <t>20191202</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>625.0</v>
+        <v>468.0</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20200428</t>
+          <t>20200327</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>523.0</v>
+        <v>666.0</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>20200617</t>
+          <t>20200402</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>620.0</v>
+        <v>526.0</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>20200416</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>625.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>20200428</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>523.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>20200617</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>620.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
           <t>20200624</t>
         </is>
       </c>
-      <c r="B59" t="n">
+      <c r="B62" t="n">
         <v>570.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add matrix up range
</commit_message>
<xml_diff>
--- a/src/main/resources/SZ300181.xlsx
+++ b/src/main/resources/SZ300181.xlsx
@@ -1191,6 +1191,56 @@
         <v>765.0</v>
       </c>
     </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>20200814</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>626.0</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>20200915</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>894.0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>20200929</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>701.0</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>20201019</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>847.0</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>20201113</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>675.0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
add matrix last point
</commit_message>
<xml_diff>
--- a/src/main/resources/SZ300181.xlsx
+++ b/src/main/resources/SZ300181.xlsx
@@ -1234,11 +1234,11 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>20201111</t>
+          <t>20201113</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>687.0</v>
+        <v>675.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add first class buy sell point
</commit_message>
<xml_diff>
--- a/src/main/resources/SZ300181.xlsx
+++ b/src/main/resources/SZ300181.xlsx
@@ -1234,11 +1234,41 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>20201113</t>
+          <t>20201211</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>675.0</v>
+        <v>605.0</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>20201222</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>653.0</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>20210108</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>539.0</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>20210329</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>736.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>